<commit_message>
Batch Put test case scenarios
Batch Put test case scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/batch_testdata.xlsx
+++ b/src/test/resources/excelData/batch_testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Vasanthi-SDET\APIMaster\7CRUDCarriers_LMS_API\7CRUDCarriers_LMS_API\src\test\resources\excelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD451C66-C3A8-4B8A-9893-1CF50BB2B28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A4B661-F71C-4E53-9325-62DD73B8B012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
   <si>
     <t>Test case Name</t>
   </si>
@@ -261,9 +261,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>Batch successfully Updated!</t>
-  </si>
-  <si>
     <t>UserId</t>
   </si>
   <si>
@@ -294,28 +291,92 @@
     <t>ABC</t>
   </si>
   <si>
+    <t>Batch Successfully Updated</t>
+  </si>
+  <si>
     <t xml:space="preserve">   {
-        "batchName": "Updated Batch by Vasanthi",
+        "batchName": "Updated Batch by Vasanthi with Batch Id",
         "batchDescription": "Selenium Training",
         "batchStatus": "Active",
         "batchNoOfClasses": 184,
-        "programId": 364,
+        "programId": 305,
         "programName": "Jan23-CRUDCarriers-SDET-4"
     }</t>
   </si>
   <si>
-    <t>To update batch with valid Batch id</t>
+    <t>To update batch with valid BatchId</t>
+  </si>
+  <si>
+    <t>Update Batch details for a invalid BatchId</t>
+  </si>
+  <si>
+    <t>609A</t>
+  </si>
+  <si>
+    <t>{
+"batchName": "Jan23-CRUDCarriers-SDET-251",
+"batchDescription": "API07",
+"batchStatus": "Active",
+"batchNoOfClasses": 13,
+"programId": 305,
+"programName": "Jan23-CRUDCarriers-SDET-009"
+}</t>
+  </si>
+  <si>
+    <t>Batch not found with Id : -609</t>
+  </si>
+  <si>
+    <t>Unsupported Media Type</t>
+  </si>
+  <si>
+    <t>Update Batch details with Alphanumeric BatchId</t>
+  </si>
+  <si>
+    <t>Update Batch details with blank BatchId</t>
+  </si>
+  <si>
+    <t>Update Batch details with decimal BatchId</t>
+  </si>
+  <si>
+    <t>Update Batch details with Negative BatchId</t>
+  </si>
+  <si>
+    <t>Update batch with valid BatchId and without JSON Schema</t>
+  </si>
+  <si>
+    <t>Method Not Allowed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -335,12 +396,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -356,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -394,52 +449,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,7 +803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C988"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6926,7 +7073,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -6937,44 +7084,44 @@
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="C4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8026,53 +8173,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA204922-E000-4942-AD84-4D5975F4154D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="12" customFormat="1" ht="118.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17">
+        <v>609</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="22">
+        <v>609999</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="18">
+        <v>400</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="19">
+        <v>400</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="20">
+        <v>405</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="24">
+        <v>609.1</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="20">
+        <v>400</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="24">
+        <v>-609</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20">
+        <v>400</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="24">
+        <v>609</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="20">
+        <v>415</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>